<commit_message>
did merge two sorted LL problem
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -1429,7 +1429,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1492,9 +1492,32 @@
         <v>Yes</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>08/11/2025</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Merge Two Sorted Linked Lists</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Linked List</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Easy</v>
+      </c>
+      <c r="E3" t="str">
+        <v>No (knew method but didnt know how to code it)</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
did linked list cycle detection leetcode
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -1429,7 +1429,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1515,9 +1515,144 @@
         <v>Yes</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>08/12/2025</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Linked List Cycle Detection</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Linked List</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Easy</v>
+      </c>
+      <c r="E4" t="str">
+        <v>No (needed hint but was able to do code)</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="str">
+        <v>Reorder List</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Linked List</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="str">
+        <v>Remove Nth Node From End of List</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Linked List</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="str">
+        <v>Copy List with Random Pointer</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Linked List</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="str">
+        <v>Add Two Numbers</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Linked List</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="str">
+        <v>Find The Duplicate Number</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Linked List</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="str">
+        <v>LRU Cache</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Linked List</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="str">
+        <v>Merge K Sorted Lists</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Linked List</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Hard</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="str">
+        <v>Reverse Nodes In K Group</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Linked List</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Hard</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
did some leetcode to practice for oa
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Binary Search" sheetId="4" r:id="rId4"/>
     <sheet name="Sliding Window" sheetId="5" r:id="rId5"/>
     <sheet name="Linked List" sheetId="6" r:id="rId6"/>
+    <sheet name="Others" sheetId="7" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -402,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -649,9 +650,55 @@
         <v>No</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>08/14/2025</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Triple ZigZag</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Arrays</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Easy</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Maybe</v>
+      </c>
+      <c r="G13" t="str">
+        <v>Yes_x000d_</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>08/14/2025</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Simple Bank System</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Arrays</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Maybe</v>
+      </c>
+      <c r="G14" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K14"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1655,4 +1702,53 @@
     <ignoredError numberStoredAsText="1" sqref="A1:K12"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Date Solved</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Algorithm</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Difficulty</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Solved First Time</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Revisit?</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Understand?</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Revisit Date #1</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Revisit Date #2</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Revisit Date #3</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Confidence Now</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:K1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
did two leetcodes for linked lists
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -1586,6 +1586,9 @@
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="str">
+        <v>08/17/2025</v>
+      </c>
       <c r="B5" t="str">
         <v>Reorder List</v>
       </c>
@@ -1595,11 +1598,20 @@
       <c r="D5" t="str">
         <v>Medium</v>
       </c>
+      <c r="E5" t="str">
+        <v>Yes (maybe needed help with optimal or code but knew the concept)</v>
+      </c>
       <c r="F5" t="str">
         <v>Yes</v>
       </c>
+      <c r="G5" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="6">
+      <c r="A6" t="str">
+        <v>08/17/2025</v>
+      </c>
       <c r="B6" t="str">
         <v>Remove Nth Node From End of List</v>
       </c>
@@ -1609,7 +1621,13 @@
       <c r="D6" t="str">
         <v>Medium</v>
       </c>
+      <c r="E6" t="str">
+        <v>Yes (only needed help with error in brute but needed help in optimal)</v>
+      </c>
       <c r="F6" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G6" t="str">
         <v>Yes</v>
       </c>
     </row>

</xml_diff>

<commit_message>
did leetcode copy LL with random pointers
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -1632,6 +1632,9 @@
       </c>
     </row>
     <row r="7">
+      <c r="A7" t="str">
+        <v>08/19/2025</v>
+      </c>
       <c r="B7" t="str">
         <v>Copy List with Random Pointer</v>
       </c>
@@ -1641,7 +1644,13 @@
       <c r="D7" t="str">
         <v>Medium</v>
       </c>
+      <c r="E7" t="str">
+        <v>No</v>
+      </c>
       <c r="F7" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G7" t="str">
         <v>Yes</v>
       </c>
     </row>

</xml_diff>

<commit_message>
did add two numbers LL problem
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -1655,6 +1655,9 @@
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="str">
+        <v>08/24/2025</v>
+      </c>
       <c r="B8" t="str">
         <v>Add Two Numbers</v>
       </c>
@@ -1664,7 +1667,13 @@
       <c r="D8" t="str">
         <v>Medium</v>
       </c>
+      <c r="E8" t="str">
+        <v>Somewhat (managed to come up with a solution but didnt work fully so had to look at correct tutorial)</v>
+      </c>
       <c r="F8" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G8" t="str">
         <v>Yes</v>
       </c>
     </row>

</xml_diff>

<commit_message>
did two linked list leetcode problems
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -1678,6 +1678,9 @@
       </c>
     </row>
     <row r="9">
+      <c r="A9" t="str">
+        <v>08/25/2025</v>
+      </c>
       <c r="B9" t="str">
         <v>Find The Duplicate Number</v>
       </c>
@@ -1687,7 +1690,13 @@
       <c r="D9" t="str">
         <v>Medium</v>
       </c>
+      <c r="E9" t="str">
+        <v>Yes (did O(n) time and space but looked up better space  complexity)</v>
+      </c>
       <c r="F9" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G9" t="str">
         <v>Yes</v>
       </c>
     </row>

</xml_diff>

<commit_message>
did 2 more leetcode
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -1701,6 +1701,9 @@
       </c>
     </row>
     <row r="10">
+      <c r="A10" t="str">
+        <v>08/27/2025</v>
+      </c>
       <c r="B10" t="str">
         <v>LRU Cache</v>
       </c>
@@ -1710,11 +1713,20 @@
       <c r="D10" t="str">
         <v>Medium</v>
       </c>
+      <c r="E10" t="str">
+        <v>Somewhat</v>
+      </c>
       <c r="F10" t="str">
         <v>Yes</v>
       </c>
+      <c r="G10" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="11">
+      <c r="A11" t="str">
+        <v>08/30/2025</v>
+      </c>
       <c r="B11" t="str">
         <v>Merge K Sorted Lists</v>
       </c>
@@ -1724,11 +1736,20 @@
       <c r="D11" t="str">
         <v>Hard</v>
       </c>
+      <c r="E11" t="str">
+        <v>No</v>
+      </c>
       <c r="F11" t="str">
         <v>Yes</v>
       </c>
+      <c r="G11" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="12">
+      <c r="A12" t="str">
+        <v>08/30/2025</v>
+      </c>
       <c r="B12" t="str">
         <v>Reverse Nodes In K Group</v>
       </c>
@@ -1738,7 +1759,13 @@
       <c r="D12" t="str">
         <v>Hard</v>
       </c>
+      <c r="E12" t="str">
+        <v>No</v>
+      </c>
       <c r="F12" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G12" t="str">
         <v>Yes</v>
       </c>
     </row>

</xml_diff>

<commit_message>
leetcode same binary tree problem
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Binary Search" sheetId="4" r:id="rId4"/>
     <sheet name="Sliding Window" sheetId="5" r:id="rId5"/>
     <sheet name="Linked List" sheetId="6" r:id="rId6"/>
-    <sheet name="Others" sheetId="7" r:id="rId7"/>
+    <sheet name="Trees" sheetId="7" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -1778,7 +1778,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1818,9 +1818,270 @@
         <v>Confidence Now</v>
       </c>
     </row>
+    <row r="2">
+      <c r="B2" t="str">
+        <v>Invert Binary Tree</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Easy</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="str">
+        <v>Maximum Depth of Binary Tree</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Easy</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="str">
+        <v>Diameter of Binary Tree</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Easy</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="str">
+        <v>Balanced Binary Tree</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Easy</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>08/31/2025</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Same Tree</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Easy</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="str">
+        <v>Subtree of Another Tree</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Easy</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="str">
+        <v>Lowest Common Ancestor of a Binary Search Tree</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="str">
+        <v>Binary Tree Level Order Traversal</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="str">
+        <v>Binary Tree Right Side View</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G10" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="str">
+        <v>Count Good Nodes in Binary Tree</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G11" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="str">
+        <v>Validate Binary Search Tree</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G12" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="str">
+        <v>Kth Smallest Element in a Bst</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G13" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="str">
+        <v>Construct Binary Tree From Preorder and Inorder Traversal</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G14" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="str">
+        <v>Binary Tree Maximum Path Sum</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Hard</v>
+      </c>
+      <c r="F15" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="str">
+        <v>Serialize and Deserialize Binary Tree</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Trees</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Hard</v>
+      </c>
+      <c r="F16" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="G16" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K16"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
did 2 tree leetcodes
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -1836,6 +1836,9 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="str">
+        <v>09/03/2025</v>
+      </c>
       <c r="B3" t="str">
         <v>Maximum Depth of Binary Tree</v>
       </c>
@@ -1844,6 +1847,9 @@
       </c>
       <c r="D3" t="str">
         <v>Easy</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Yes</v>
       </c>
       <c r="F3" t="str">
         <v>Yes</v>
@@ -1870,6 +1876,9 @@
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="str">
+        <v>09/03/2025</v>
+      </c>
       <c r="B5" t="str">
         <v>Balanced Binary Tree</v>
       </c>
@@ -1878,6 +1887,9 @@
       </c>
       <c r="D5" t="str">
         <v>Easy</v>
+      </c>
+      <c r="E5" t="str">
+        <v>No</v>
       </c>
       <c r="F5" t="str">
         <v>Yes</v>

</xml_diff>

<commit_message>
did 2 more leetcode tree (super busy couple of weeks but should be good now)
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -1868,6 +1868,9 @@
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="str">
+        <v>09/16/2025</v>
+      </c>
       <c r="B4" t="str">
         <v>Diameter of Binary Tree</v>
       </c>
@@ -1876,6 +1879,9 @@
       </c>
       <c r="D4" t="str">
         <v>Easy</v>
+      </c>
+      <c r="E4" t="str">
+        <v>No</v>
       </c>
       <c r="F4" t="str">
         <v>Yes</v>
@@ -1931,6 +1937,9 @@
       </c>
     </row>
     <row r="7">
+      <c r="A7" t="str">
+        <v>09/16/2025</v>
+      </c>
       <c r="B7" t="str">
         <v>Subtree of Another Tree</v>
       </c>

</xml_diff>

<commit_message>
did 1 leetcode medium 1 hard for trees
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -2006,6 +2006,9 @@
       </c>
     </row>
     <row r="10">
+      <c r="A10" t="str">
+        <v>09/22/2025</v>
+      </c>
       <c r="B10" t="str">
         <v>Binary Tree Right Side View</v>
       </c>
@@ -2014,6 +2017,9 @@
       </c>
       <c r="D10" t="str">
         <v>Medium</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Kinda (needed some help but had somewhat the right idea and code)</v>
       </c>
       <c r="F10" t="str">
         <v>Yes</v>
@@ -2120,6 +2126,9 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" t="str">
+        <v>09/22/2025</v>
+      </c>
       <c r="B16" t="str">
         <v>Serialize and Deserialize Binary Tree</v>
       </c>
@@ -2128,6 +2137,9 @@
       </c>
       <c r="D16" t="str">
         <v>Hard</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Kinda (figured out serialization and thought it was wrong because of the output eventhough it wasnt. made me look for help when I should have kept going)</v>
       </c>
       <c r="F16" t="str">
         <v>Yes</v>

</xml_diff>

<commit_message>
did 1 leetcode finished trees
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -2122,6 +2122,9 @@
       </c>
     </row>
     <row r="14">
+      <c r="A14" t="str">
+        <v>09/24/2025</v>
+      </c>
       <c r="B14" t="str">
         <v>Construct Binary Tree From Preorder and Inorder Traversal</v>
       </c>
@@ -2130,6 +2133,12 @@
       </c>
       <c r="D14" t="str">
         <v>Medium</v>
+      </c>
+      <c r="E14" t="str">
+        <v>No</v>
+      </c>
+      <c r="F14" t="str">
+        <v>https://www.youtube.com/watch?v=ihj4IQGZ2zc  ||    https://www.youtube.com/watch?v=PbPS460rbMo</v>
       </c>
       <c r="G14" t="str">
         <v>Yes</v>

</xml_diff>

<commit_message>
did leetcode and freecodecamp full stack
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sliding Window" sheetId="5" r:id="rId5"/>
     <sheet name="Linked List" sheetId="6" r:id="rId6"/>
     <sheet name="Trees" sheetId="7" r:id="rId7"/>
+    <sheet name="Tries" sheetId="8" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -2224,4 +2225,107 @@
     <ignoredError numberStoredAsText="1" sqref="A1:L18"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Date Solved</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Algorithm</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Difficulty</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Solved First Time</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Video Help</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Revisit?</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Understand?</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Revisit Date #1</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Revisit Date #2</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Revisit Date #3</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Confidence Now</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>09/30/25</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Implement Trie Prefix Tree</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Tries</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Kinda</v>
+      </c>
+      <c r="F2" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Maybe</v>
+      </c>
+      <c r="H2" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <v>Design Add and Search Words Data Structure</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Tries</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Medium</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="str">
+        <v>Word Search 2</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Tries</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Hard</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
did 2 leetcode heap problems
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -2491,6 +2491,9 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="str">
+        <v>10/9/25</v>
+      </c>
       <c r="B3" t="str">
         <v>Last Stone Weight</v>
       </c>
@@ -2500,8 +2503,20 @@
       <c r="D3" t="str">
         <v>Easy</v>
       </c>
+      <c r="E3" t="str">
+        <v>Yes (but theres a more complex/faster bucket sort version)</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Yes</v>
+      </c>
     </row>
     <row r="4">
+      <c r="A4" t="str">
+        <v>10/9/25</v>
+      </c>
       <c r="B4" t="str">
         <v>K Closest Points to Origin</v>
       </c>
@@ -2510,6 +2525,18 @@
       </c>
       <c r="D4" t="str">
         <v>Medium</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Kinda (struggled with coding the comparator)</v>
+      </c>
+      <c r="F4" t="str">
+        <v>https://youtu.be/rI2EBUEMfTk</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="H4" t="str">
+        <v>Yes</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
1 backtracking leetcode (monitor broke only have 1 bad monitor rn)
</commit_message>
<xml_diff>
--- a/NeetCode150/LeetCodeTracker.xlsx
+++ b/NeetCode150/LeetCodeTracker.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Trees" sheetId="7" r:id="rId7"/>
     <sheet name="Tries" sheetId="8" r:id="rId8"/>
     <sheet name="Heap" sheetId="9" r:id="rId9"/>
+    <sheet name="Backtracking" sheetId="10" r:id="rId10"/>
   </sheets>
 </workbook>
 </file>
@@ -727,6 +728,160 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Date Solved</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Algorithm</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Difficulty</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Solved First Time</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Video Help</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Revisit?</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Understand?</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Revisit Date #1</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Revisit Date #2</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Revisit Date #3</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Confidence Now</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>10/24/25</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Subsets</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Backtracking</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Medium</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="str">
+        <v>Combination Sum</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Backtracking</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Medium</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="str">
+        <v>Combination Sum 2</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Backtracking</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Medium</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="str">
+        <v>Permutations</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Backtracking</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Medium</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="str">
+        <v>Subsets 2</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Backtracking</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Medium</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="str">
+        <v>Word Search</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Backtracking</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Medium</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="str">
+        <v>Palindrome Partitioning</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Backtracking</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Medium</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="str">
+        <v>Letter Combinations of a Phone Number</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Backtracking</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Medium</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="str">
+        <v>N Queens</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Backtracking</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Hard</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:L10"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L6"/>

</xml_diff>